<commit_message>
Docker Network with PgDb and PgAdmin
</commit_message>
<xml_diff>
--- a/Work Tracking.xlsx
+++ b/Work Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SANYA\Documents\PersonalProjects\Zoomcamp\data-engineering-zoomcamp-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD16D14F-8669-490E-B059-90B9F95B14DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7060E47-D7B1-4131-9CA5-BE138DA0803B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>Week Number</t>
   </si>
@@ -86,739 +86,25 @@
     <t>Logging daily work and todolist</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Current Version on my system: Spacy - 2.1.3 &amp; en_core_web_lg model - 2.1.0 || Latest Version available: Spacy - 2.3.0 &amp; en_core_web_lg - 2.3.0 </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Documentation: Checking for newer versions of Spacy</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Todo: Go through the queuing system, DM App. Readup on the changes in the new server.  </t>
-  </si>
-  <si>
-    <t>Tried connecting to the Git repo via Gitbash but got a message that the SSL Certificate has expired. Checked the security groups on AWS but could not find the name of the dev server. Need to find out the name of the Dev server, check if I have added myself to the right security groups and then connect to the Dev Server.</t>
-  </si>
-  <si>
     <t>Queueing System: Familiarize myself to this new way of processing sentences by looking at the code in GitLab</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Found the repositiories and the files of interest.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Studying the changes in the ner_spacy model (Iteration 1) Studying the changes (Iteration 2) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Meeting with Rod</t>
-    </r>
   </si>
   <si>
     <t>Dev Server</t>
   </si>
   <si>
-    <t>Get Access to DM App (1) Refactored ner_spacy Went through the changes on the DMV3 Server; i.e. whats new in pm2 Amzon Linux</t>
-  </si>
-  <si>
-    <t>DM App Feedback document. Tranformer Model Basic Understanding</t>
-  </si>
-  <si>
     <t>NLP Research</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Read up on RNN's, LSTM &amp; GRU. Continue reading about transformers at </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://medium.com/inside-machine-learning/what-is-a-transformer-d07dd1fbec04</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Todo: I'll be dividing my time between NLP Research, Tranformer Model &amp; Instagram Project </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Done: Read up on RNN, LSTM &amp; GRU's. Completed the issues on GitLab</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Read up on RNN's, LSTM &amp; GRU.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Read about Transformers and understood the attention mechanism. Read up about the BERT model. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Found the repositiories and the files of interest</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Understood the technologies and the models used and looked at the papers referenced.</t>
-    </r>
-  </si>
-  <si>
-    <t>Todo: Transformers and Instagram Model</t>
   </si>
   <si>
     <t>NLP Research for Business Signal Identification</t>
   </si>
   <si>
-    <t>Read research papers on business signal identification from text. In simple terms sentence classification using state of the art technologies.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Read up on RNN's, LSTM &amp; GRU.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Read about Transformers and understood the attention mechanism. Read up about the BERT model.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Read up about the different types of transformer type models available -ELECTRA, RoBERTa. Read up in detail about Elecktra model and tabulated it's pros and cons. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Found the repositiories and the files of interest</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Understood the technologies and the models used and looked at the papers referenced.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Read up paper until chaper 3.</t>
-    </r>
-  </si>
-  <si>
-    <t>Done: BERT and it's versions and started looking at ELECTRA model.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Read up on RNN's, LSTM &amp; GRU.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Read about Transformers and understood the attention mechanism. Read up about the BERT model.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Read up about the different types of transformer type models available -ELECTRA, RoBERTa. Read up in detail about Elecktra model and tabulated it's pros and cons.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Read up about XLNet model and document the pros and cons.  Made a note of the datasets used by each model. T5 Model. Look at glue to find the best performing models in NLP. Read some research papers on comparison of these models. Look at implementation code</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Todo: Will continue research with the NLP research and finish the LM (Language models) I started yesterday (ELECTRA and)and then move onto new ones  XLNet, T5 Models. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Done: ELECTRA, XLNet along with some papers on these model comparisons</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Read up on RNN's, LSTM &amp; GRU.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Read about Transformers and understood the attention mechanism. Read up about the BERT model.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Read up about the different types of transformer type models available -ELECTRA, RoBERTa. Read up in detail about Elecktra model and tabulated it's pros and cons.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Read up about XLNet model and document the pros and cons.  Made a note of the datasets used by each model. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>T5 Model, looked at in detail to understand how it can be used for mutiple classification tasks. Looked at glue to find the best performing models in NLP (found StructBERT, need to find more)(2). Documented infor on StructBERT. Downloaded and analysed the AGNews dataset and decided that maybe models on this leaderboard will be more interesting to look at (as the dataset consists of sentences) and found a new model BERT-ITPT-FiT after researching what models are available (3). Todo: Read some research papers on comparison of these models. Look at implementation code.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Todo: Continue with Language Model Research. Look at GLUE BEnchmark to find state of the art LM's. Look at T5 model. Look out for more NLP models by reading some more papers on NLP Research. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Done: T5 Model in detail and looked at other models - StructBERT and  BERT -ITPT-FiT</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Read up on RNN's, LSTM &amp; GRU. Read about Transformers and understood the attention mechanism. Read up about the BERT model. Read up about the different types of transformer type models available -ELECTRA, RoBERTa. Read up in detail about Elecktra model and tabulated it's pros and cons. Read up about XLNet model and document the pros and cons.  Made a note of the datasets used by each model. T5 Model, looked at in detail to understand how it can be used for mutiple classification tasks. Looked at glue to find the best performing models in NLP (found StructBERT, need to find more)(2). Documented infor on StructBERT. Downloaded and analysed the AGNews dataset and decided that maybe models on this leaderboard will be more interesting to look at (as the dataset consists of sentences) and found a new model BERT-ITPT-FiT after researching what models are available (3). </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">This session: Went through AGNews Benchmark and found other models (1.5) UMLFit Paper (.5) </t>
-    </r>
-  </si>
-  <si>
     <t>DL Environment Setup</t>
-  </si>
-  <si>
-    <t>Investigated the free enviroments available online with access to GPU for training DL Models.(2) Meeting with Áine and Rod (.5)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Todo: AGNews Benchmark, maximum sentence length - Finish up with one of the models. Read up a couple of more research papers. Implementation Code? What platform will I be using for implementation? </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Done: Researched a new model, then I was looking at various environments available for DL. Mid way of documenting the memory requirements for each LM. </t>
-    </r>
-  </si>
-  <si>
-    <t>Researched into and documented what is the computational requirement (in terms of GPU) for training these models on our own data(2). Look at implementation code(2).</t>
-  </si>
-  <si>
-    <t>Preparation (2) Presentation (1.5)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Todo:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Completed Phase 1 of the NLP research. And consolidate and shared the results.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Did a quick overview of the language options available in T5. Could only determine that it does multi-language translation in terms of translating English to French, Germen and Romanian. Currenly it is not a language agnostic model.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Read the paper and concluded that it uses English as base language and performs text generation and downstream tasks only in English. Text classification is not tested in particular in the paper. </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Todo: Perform Phase 2 of NLU Models - T5 to be specific. </t>
-  </si>
-  <si>
-    <t>Need to read up on the language options in ELECTRA. Look into other language agnostic models.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Did a quick overview of the language options available in T5. Could only determine that it does multi-language translation in terms of translating English to French, Germen and Romanian. Currenly it is not a language agnostic model.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Read the paper and concluded that it uses English as base language and performs text generation and downstream tasks only in English. Looked quickly at the code support available online. T5 Malay, Arabic. Looked into BERT language options. Monolingual BERTs and mBERT. Text classification is not tested in particular in the paper. Need to read up on the language options in ELECTRA. Compare what is better for text classification and language support for - Electra, T5, XLNet or UMLFiT. Look into language-agnostic models? Document the findings.</t>
-    </r>
-  </si>
-  <si>
-    <t>Check the Postgres DB to find the avg sentence length.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Todo: Finish up what I had left from yesterday (T5).Then look in detail at the language options for the other models I had investigated earlier. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>DONE: Finished with T5, looking into the other models.  Then started looking at BERT language options thinking it would be straight forward but that was not the case. Then started looking into mBERT. The documentation says it's multilingual. But it wasn't clear if it does just translations or also performs downstream tasks irrespective of the language or not. Not straight forward as the language implementations are done by others and there is no one place to find them all. Also, the main task is translation so I'm having to read into the documentation to understand what the model can do and also refer to papers to verify if the performance is significant or not and if text classification is possible or not.</t>
-    </r>
-  </si>
-  <si>
-    <t>Researched mBERT and XLM-R</t>
-  </si>
-  <si>
-    <t>Reserched model mT5 (4), ELECTRA multilingual support, documentation and preparation for meeting with Áine and Duncan</t>
-  </si>
-  <si>
-    <t>Todo: Complete the research, mT5 model, finish documentation, meeting?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Went through the NER Model and Prospect Model to revise the new structure (1.5) Meeting with Rod and Documenting the meeting (3) </t>
-  </si>
-  <si>
-    <t>Looked into what is __init__.py (1) @property and how to use it(2)</t>
-  </si>
-  <si>
-    <t>Todo: Understanding queuing system, look into the new structure and understand the methodologies used. Working on the documentation for tomorrow.</t>
-  </si>
-  <si>
-    <t>Looked at what columns were utilised to understand the kind of classification that was performed.</t>
-  </si>
-  <si>
-    <t>Prepare the documentation, check the huggingface package, meeting with Duncan and Aine. Found that huggingface has not yet introduced mT5 (1) Consolidated the documentation (1) Meeting + Prep - (3)</t>
-  </si>
-  <si>
-    <t>Todo: Prepare for the meeting. If done look at the packages or Instagram Model</t>
-  </si>
-  <si>
-    <t>Looking at the modules and alternating between the documentation to understand the target domain features and labels. (4) Cloned the repo, but I think I'll probably imlement in google colab.(.5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Done: Looked at Source domains and Tasks and the Target Domains and tasks. And I was looking at the feature space and the class categories. Loading Google Colab, Hashing. Setting things up. Some teething issues </t>
-  </si>
-  <si>
-    <t>Run the scraper on Google Colab and look at the data coming through and understand the Instagram scraper. How and what data is scraped and how is the data structured. Had to spend time to understand what are decorators and class methods, instance methods and static methods. Had to handle to error caused by Instagram blocking the DM login for scraping. Found a solution by using personal Instagram account for scraping purposes.</t>
-  </si>
-  <si>
-    <t>Going through the thesis documentation to understand the main features and the kind of preprocessing it requires. Started with looking at Image preprocessing steps. (3)</t>
-  </si>
-  <si>
-    <t>Research and Setup the colab notebook, add the master dataset.</t>
-  </si>
-  <si>
-    <t>Issue with git - was trying to keep the 'Data' and 'outputs' folder structure using .gitignore and .gitkeep files. When creating these files on windows they were getting an extra .txt extension and therefore they were not being recognized. Finally decided to only keep the Data and outputs folders but ignore the contents. First installed 3.9 in the virtual evn and all the packages in it but tensor flow did not work with it. Hence changed to 3.8 and renstalled the packages in the virtual env. Started writing the script to run the live model without the jupiter notebooks. Rod advised to chnge from 3.8 to 3.7.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Installed 3.7.9 and all the packages. NLTK_DATA issue. Ealier was getting captured by the %%capture magic command. Even the 'quiet=True' argument did not solve the error. So for now just letting it be as it's not affecting the functionality. Loaded the model that was saved. Had several errors - Path issues and then PathPosix error. Now the chrome driver error. </t>
-  </si>
-  <si>
-    <t>Solved the chrome driver path error and was able to fix a few more bugs and get the scraper running. Had issues with capturing the output of the evaluation model as it is a custom object. Trying to find a way to direct the output to a csv. Instagram scraper issue: continuing to scrape without logging in.</t>
-  </si>
-  <si>
-    <t>Have the model loaded and the scraper scraping data. Solved the problem of TF displaying GPU error messages. Could not solve the problem of nltk.download() printing to terminal. Todo: Record time - loading, scraping and prediction. Clean the code and restructure it using classes? Remove unnecessary directories.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Had to change the structure of the code to implement multi-threading. Making the code more modular by adding classes. Some errors due to warnings being displayed. Need to fix those </t>
-  </si>
-  <si>
-    <t>Worked on catching some errors due to missing data i.e. no posts or no profile. Added logging. Removed files that are not required. Fixed the Xpath for image retrieval from Insta.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Added command prompt input using the argparse module to take the input (profile names via the command line. Performed the final tests. Blocker: The tests started fialing and was returning that no Instagram profiles could be found for almost all the inputs. Tried to revert back to previous stable state and perform tests again. Checked the code and then later found out through the head-on state that Insagram was blocking login. (3) </t>
-  </si>
-  <si>
-    <t>Add the spacy documentation to DM GitLab</t>
   </si>
   <si>
     <t>ELECTRA</t>
   </si>
   <si>
-    <t>Start initial setup of the project with connection to repo via google colab. Research and find examples for implementation of ELECTRA model. Today I was able to setup the repo for the project and connect it to a temporary remote repo on GitLab. I should now be able to work on the project both from local and collab as required. Once decided on the project, I’ll use the repo you’ve created but for now I was thinking of working on this temporary repo I’ve created. I’ve shared that repo with you as well, let me know if you haven’t received my invitation. I’ll be performing basic testing on this in regards to the ELECKTRA model. After that I started to investigate some example implementations to understand what packages will be required and what is the potential environment I’ll need to create.</t>
-  </si>
-  <si>
-    <t>Had issues reconnecting to the repo. Found that that ssh keys were lost when the session changed. Came up with a work around to sole this issue by sving the keys in the drive and then copying them to the root folder before each session, connect to git and then delete them from the root after each session. This is an issue becuase people do not use GoogleColab very frequently with a private repo like GitLab. And the hack that has been mentioned t connect to a private repo was for cloaning only and therefore they do not talk or discuss about losing the ssh keys for later connectivity. As long as the session is active which is usually 90 mins the assigned server remains the same, therefore when I tested this earlier by disconnecting and reconnecting to Colab and looing up the keys and  testing the GitLab connection it worked but when I logged back in today the keys were missing. (3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Looked at conda and istalled conda. Lokked at examples of ELECTRA model but found only 1 example which was using a custom package called simpletransformers. Need to look for more examples. (3)</t>
-  </si>
-  <si>
-    <t>Install conda and setup the environment by installing required packages</t>
-  </si>
-  <si>
-    <t>Did a quick setup on colab and ran an example code</t>
-  </si>
-  <si>
-    <t>Look at codes to understand the preprocessing pipeline for ELECTRA. Looked at doms code (2) Looked at the process of cleaning the text, tokenization and encoding. Found the tokenizer for electra model. Iteration 1 (need to go trough them again to understand it completely and in association with one another)</t>
-  </si>
-  <si>
-    <t>Looked at the [SEP], [CLS] and [UNK] tokens of ELECTRA and how they need to be placed and used. (2)  Went through the preprocessing steps of description in the instagram model. (4) TODO: Understand the process_aux_text_data() function in the preprocessor module. Mainly looking at and understanding the encoding performed. Understand the make_dataset() and split_and_batch(dataset) functions by looking in detail at the tf.data.Dataset.from_tensor_slices() , batching in tf. Followed by understanding the models module in the instagram project.</t>
-  </si>
-  <si>
-    <t>Looked at the TF tutorials and tried to understand what are tensors and the Dataset classs</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Added the 'TFElectra' model to the bert_model.py module to be able to load an ELECTRA model and the ELECTRA model Tokenizer to </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>bert_text_preprocessor.py</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">. The MAIN function contains the implementations. </t>
-    </r>
-  </si>
-  <si>
     <t>YouTube</t>
-  </si>
-  <si>
-    <t>Could not find any attributes with that info.</t>
-  </si>
-  <si>
-    <t>Extracted channel ids (which are in the source of the page) and pulled videos based on just the channelID. Then extracted the videoIds and pulled the data for all those 25 videos.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pulled the videoIds from Kavitas dataset (370 examples) and then made API calls to pull data for those videos in a batch fashion as the maximum videoIds that could be sent in 1 call was 50. </t>
-  </si>
-  <si>
-    <t>Mapped the extracted data to the instagram format and add the labels to the data by making a join on videoIds. Then run the data through the instagram model and evaluate the results.</t>
-  </si>
-  <si>
-    <t>Evaluate the prediction results produced by Instarget on YouTube data. Looked in detail at the specificity, sensitivity, fscore. Then analysed in detail the examples that were misclassified. Presented all this information in a python notebook for easy viewing by other members of DM.</t>
-  </si>
-  <si>
-    <t>While analysing the results it was observed that there were errors in the prediction due to duplicated which were introduced due to some videos having diffirent video ids but same content. This would effect the evaluation results of the model. ~Hence this was cleaned and the model was rerun on the cleaned data and the results were presented in a Python notebook.For Aine to be able to view this notbook. This notebook was made available on Google Colab as well. For the purpose of presentation and ease of viewing the results, the thumbnails of the videos and a link to the videos was added to the df.</t>
-  </si>
-  <si>
-    <t>Re-looked at the data available through the Youtube v3 API to find more relavant data that we can use for building a new ELECTRA based YouTube model. Earlier I had only looked at what data we can pull for Instarget.; but now I looked into what is unique to YouTube and what we can use for the new prediction model.</t>
-  </si>
-  <si>
-    <t>Prepared code to be able to load the text model, preprocess only the textual data and run it through the Roberta model and then evaluate the results.</t>
-  </si>
-  <si>
-    <t>Bring the Roberta model in a deployment format so one post/video is labelled at a time. Added YouTube data acquisition information to .md file.</t>
-  </si>
-  <si>
-    <t>Go through the full pipeline and understand how the modelling works.  test if further cleaning of the YouTube description data before it is fed into the model(s) improves accuracy or not.</t>
-  </si>
-  <si>
-    <t>FURLOUGH</t>
   </si>
   <si>
     <t>ner_spacy model</t>
@@ -923,7 +209,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -980,19 +266,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1318,7 +591,7 @@
   <dimension ref="A1:X1084"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1348,7 +621,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1371,19 +644,19 @@
     </row>
     <row r="2" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="D2" s="5" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>109</v>
+        <v>36</v>
       </c>
       <c r="F2" s="6"/>
     </row>
@@ -1391,13 +664,13 @@
       <c r="A3" s="2"/>
       <c r="B3" s="7"/>
       <c r="C3" s="4" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="D3" s="5" t="b">
         <v>0</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>112</v>
+        <v>39</v>
       </c>
       <c r="F3" s="6"/>
     </row>
@@ -1405,13 +678,13 @@
       <c r="A4" s="2"/>
       <c r="B4" s="7"/>
       <c r="C4" s="4" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="D4" s="5" t="b">
         <v>0</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
       <c r="F4" s="6"/>
     </row>
@@ -1425,7 +698,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="F5" s="6"/>
     </row>
@@ -1493,236 +766,140 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>2</v>
-      </c>
-      <c r="B14" s="3">
-        <v>44109</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>16</v>
-      </c>
+    <row r="14" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="5" t="b">
-        <v>1</v>
-      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="7"/>
-      <c r="C17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>2</v>
-      </c>
-      <c r="B18" s="3">
-        <v>44110</v>
-      </c>
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D18" s="5"/>
       <c r="E18" s="10"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
       <c r="B21" s="7"/>
-      <c r="C21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:24" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="7"/>
-      <c r="C22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="7"/>
-      <c r="C23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="6"/>
-      <c r="F23" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
-        <v>2</v>
-      </c>
-      <c r="B24" s="3">
-        <v>44111</v>
-      </c>
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D24" s="5"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="7"/>
-      <c r="C25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="5" t="b">
-        <v>1</v>
-      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="7"/>
-      <c r="C26" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="8"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:24" ht="57" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="7"/>
-      <c r="C27" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="5"/>
       <c r="E27" s="6"/>
-      <c r="F27" s="13" t="s">
-        <v>26</v>
-      </c>
+      <c r="F27" s="13"/>
     </row>
     <row r="28" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="7"/>
-      <c r="C28" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <v>2</v>
-      </c>
-      <c r="B29" s="3">
-        <v>44112</v>
-      </c>
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D29" s="5"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="14"/>
-      <c r="C30" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="6"/>
       <c r="F30" s="4"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
@@ -1743,86 +920,52 @@
       <c r="W30" s="5"/>
       <c r="X30" s="5"/>
     </row>
-    <row r="31" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="7"/>
-      <c r="C31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="7"/>
-      <c r="C32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="6"/>
-      <c r="F32" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="5"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
     <row r="34" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
-        <v>3</v>
-      </c>
-      <c r="B34" s="3">
-        <v>44116</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D34" s="5"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="7"/>
-      <c r="C35" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:24" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
       <c r="B36" s="14"/>
-      <c r="C36" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="6"/>
       <c r="F36" s="4"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
@@ -1843,72 +986,44 @@
       <c r="W36" s="5"/>
       <c r="X36" s="5"/>
     </row>
-    <row r="37" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="7"/>
-      <c r="C37" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="7"/>
-      <c r="C38" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="5"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="F38" s="6"/>
     </row>
     <row r="39" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="7"/>
-      <c r="C39" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
     <row r="40" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
-        <v>3</v>
-      </c>
-      <c r="B40" s="3">
-        <v>44117</v>
-      </c>
+      <c r="A40" s="2"/>
+      <c r="B40" s="3"/>
       <c r="C40" s="4"/>
-      <c r="D40" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D40" s="5"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:24" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
       <c r="B41" s="14"/>
-      <c r="C41" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="6"/>
       <c r="F41" s="4"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
@@ -1929,58 +1044,36 @@
       <c r="W41" s="5"/>
       <c r="X41" s="5"/>
     </row>
-    <row r="42" spans="1:24" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="7"/>
-      <c r="C42" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D42" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="6"/>
-      <c r="F42" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="7"/>
-      <c r="C43" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="5"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
     <row r="44" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
-        <v>3</v>
-      </c>
-      <c r="B44" s="3">
-        <v>44118</v>
-      </c>
+      <c r="A44" s="2"/>
+      <c r="B44" s="3"/>
       <c r="C44" s="4"/>
-      <c r="D44" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D44" s="5"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:24" ht="102" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
       <c r="B45" s="14"/>
-      <c r="C45" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="6"/>
       <c r="F45" s="4"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
@@ -2001,58 +1094,36 @@
       <c r="W45" s="5"/>
       <c r="X45" s="5"/>
     </row>
-    <row r="46" spans="1:24" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="7"/>
-      <c r="C46" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C46" s="4"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="6"/>
-      <c r="F46" s="13" t="s">
-        <v>38</v>
-      </c>
+      <c r="F46" s="13"/>
     </row>
     <row r="47" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="7"/>
-      <c r="C47" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C47" s="4"/>
+      <c r="D47" s="5"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
     <row r="48" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
-        <v>3</v>
-      </c>
-      <c r="B48" s="3">
-        <v>44119</v>
-      </c>
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
       <c r="C48" s="4"/>
-      <c r="D48" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D48" s="5"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:24" ht="102" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="5"/>
       <c r="B49" s="14"/>
-      <c r="C49" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D49" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="C49" s="4"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="6"/>
       <c r="F49" s="4"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
@@ -2076,15 +1147,9 @@
     <row r="50" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
       <c r="B50" s="14"/>
-      <c r="C50" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D50" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="6"/>
       <c r="F50" s="4"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
@@ -2105,201 +1170,123 @@
       <c r="W50" s="5"/>
       <c r="X50" s="5"/>
     </row>
-    <row r="51" spans="1:24" ht="114" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="7"/>
-      <c r="C51" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D51" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C51" s="4"/>
+      <c r="D51" s="5"/>
       <c r="E51" s="6"/>
-      <c r="F51" s="13" t="s">
-        <v>42</v>
-      </c>
+      <c r="F51" s="13"/>
     </row>
     <row r="52" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="7"/>
-      <c r="C52" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C52" s="4"/>
+      <c r="D52" s="5"/>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
     </row>
     <row r="53" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A53" s="2">
-        <v>4</v>
-      </c>
-      <c r="B53" s="3">
-        <v>44123</v>
-      </c>
+      <c r="A53" s="2"/>
+      <c r="B53" s="3"/>
       <c r="C53" s="4"/>
-      <c r="D53" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D53" s="5"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
     </row>
     <row r="54" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="3"/>
-      <c r="C54" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D54" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C54" s="4"/>
+      <c r="D54" s="5"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="3"/>
-      <c r="C55" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D55" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="C55" s="4"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="6"/>
       <c r="F55" s="6"/>
     </row>
     <row r="56" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="3"/>
-      <c r="C56" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D56" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>44</v>
-      </c>
+      <c r="C56" s="4"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="6"/>
       <c r="F56" s="6"/>
     </row>
     <row r="57" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="7"/>
-      <c r="C57" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D57" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C57" s="4"/>
+      <c r="D57" s="5"/>
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="7"/>
-      <c r="C58" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C58" s="4"/>
+      <c r="D58" s="5"/>
       <c r="E58" s="6"/>
-      <c r="F58" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="F58" s="6"/>
     </row>
     <row r="59" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A59" s="2">
-        <v>4</v>
-      </c>
-      <c r="B59" s="3">
-        <v>44124</v>
-      </c>
+      <c r="A59" s="2"/>
+      <c r="B59" s="3"/>
       <c r="C59" s="4"/>
-      <c r="D59" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D59" s="5"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
     </row>
     <row r="60" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="3"/>
-      <c r="C60" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D60" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C60" s="4"/>
+      <c r="D60" s="5"/>
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="3"/>
-      <c r="C61" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D61" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>46</v>
-      </c>
+      <c r="C61" s="4"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="6"/>
       <c r="F61" s="6"/>
     </row>
     <row r="62" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="7"/>
-      <c r="C62" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D62" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C62" s="4"/>
+      <c r="D62" s="5"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="7"/>
-      <c r="C63" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C63" s="4"/>
+      <c r="D63" s="5"/>
       <c r="E63" s="6"/>
-      <c r="F63" s="6" t="s">
-        <v>47</v>
-      </c>
+      <c r="F63" s="6"/>
     </row>
     <row r="64" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A64" s="2">
-        <v>4</v>
-      </c>
-      <c r="B64" s="3">
-        <v>44125</v>
-      </c>
+      <c r="A64" s="2"/>
+      <c r="B64" s="3"/>
       <c r="C64" s="4"/>
-      <c r="D64" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D64" s="5"/>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
     </row>
     <row r="65" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="7"/>
-      <c r="C65" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D65" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C65" s="4"/>
+      <c r="D65" s="5"/>
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
     </row>
@@ -2307,324 +1294,192 @@
       <c r="A66" s="2"/>
       <c r="B66" s="7"/>
       <c r="C66" s="4"/>
-      <c r="D66" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="16" t="s">
-        <v>48</v>
-      </c>
+      <c r="D66" s="5"/>
+      <c r="E66" s="16"/>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
-      <c r="C67" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D67" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="C67" s="4"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="6"/>
       <c r="F67" s="6"/>
     </row>
     <row r="68" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="3"/>
-      <c r="C68" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D68" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="C68" s="4"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="6"/>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="7"/>
-      <c r="C69" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D69" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C69" s="4"/>
+      <c r="D69" s="5"/>
       <c r="E69" s="6"/>
-      <c r="F69" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="F69" s="6"/>
     </row>
     <row r="70" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A70" s="2">
-        <v>4</v>
-      </c>
-      <c r="B70" s="3">
-        <v>44126</v>
-      </c>
+      <c r="A70" s="2"/>
+      <c r="B70" s="3"/>
       <c r="C70" s="4"/>
-      <c r="D70" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D70" s="5"/>
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
     </row>
     <row r="71" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
-      <c r="C71" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D71" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="C71" s="4"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="6"/>
       <c r="F71" s="6"/>
     </row>
     <row r="72" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="7"/>
-      <c r="C72" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D72" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C72" s="4"/>
+      <c r="D72" s="5"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
     </row>
     <row r="73" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="7"/>
-      <c r="C73" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D73" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C73" s="4"/>
+      <c r="D73" s="5"/>
       <c r="E73" s="6"/>
       <c r="F73" s="4"/>
     </row>
     <row r="74" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A74" s="2">
-        <v>5</v>
-      </c>
-      <c r="B74" s="3">
-        <v>44130</v>
-      </c>
+      <c r="A74" s="2"/>
+      <c r="B74" s="3"/>
       <c r="C74" s="4"/>
-      <c r="D74" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D74" s="5"/>
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
     </row>
     <row r="75" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="3"/>
-      <c r="C75" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D75" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="C75" s="4"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="6"/>
       <c r="F75" s="6"/>
     </row>
     <row r="76" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="7"/>
-      <c r="C76" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D76" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C76" s="4"/>
+      <c r="D76" s="5"/>
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="7"/>
-      <c r="C77" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D77" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C77" s="4"/>
+      <c r="D77" s="5"/>
       <c r="E77" s="6"/>
-      <c r="F77" s="6" t="s">
-        <v>54</v>
-      </c>
+      <c r="F77" s="6"/>
     </row>
     <row r="78" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A78" s="2">
-        <v>5</v>
-      </c>
-      <c r="B78" s="3">
-        <v>44131</v>
-      </c>
+      <c r="A78" s="2"/>
+      <c r="B78" s="3"/>
       <c r="C78" s="4"/>
-      <c r="D78" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D78" s="5"/>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
     </row>
-    <row r="79" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="3"/>
-      <c r="C79" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D79" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="C79" s="13"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="6"/>
       <c r="F79" s="6"/>
     </row>
     <row r="80" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="3"/>
-      <c r="C80" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D80" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>56</v>
-      </c>
+      <c r="C80" s="13"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="6"/>
       <c r="F80" s="6"/>
     </row>
     <row r="81" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="7"/>
-      <c r="C81" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D81" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C81" s="4"/>
+      <c r="D81" s="5"/>
       <c r="E81" s="6"/>
       <c r="F81" s="6"/>
     </row>
-    <row r="82" spans="1:24" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="7"/>
-      <c r="C82" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D82" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C82" s="4"/>
+      <c r="D82" s="5"/>
       <c r="E82" s="6"/>
-      <c r="F82" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="F82" s="6"/>
     </row>
     <row r="83" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A83" s="2">
-        <v>5</v>
-      </c>
-      <c r="B83" s="3">
-        <v>44132</v>
-      </c>
+      <c r="A83" s="2"/>
+      <c r="B83" s="3"/>
       <c r="C83" s="4"/>
-      <c r="D83" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D83" s="5"/>
       <c r="E83" s="6"/>
       <c r="F83" s="6"/>
     </row>
     <row r="84" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="3"/>
-      <c r="C84" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D84" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>58</v>
-      </c>
+      <c r="C84" s="13"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="6"/>
       <c r="F84" s="6"/>
     </row>
-    <row r="85" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="3"/>
-      <c r="C85" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D85" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>59</v>
-      </c>
+      <c r="C85" s="4"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="6"/>
       <c r="F85" s="6"/>
     </row>
     <row r="86" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="7"/>
-      <c r="C86" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D86" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C86" s="4"/>
+      <c r="D86" s="5"/>
       <c r="E86" s="6"/>
       <c r="F86" s="6"/>
     </row>
-    <row r="87" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="7"/>
-      <c r="C87" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D87" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C87" s="4"/>
+      <c r="D87" s="5"/>
       <c r="E87" s="6"/>
-      <c r="F87" s="13" t="s">
-        <v>60</v>
-      </c>
+      <c r="F87" s="13"/>
     </row>
     <row r="88" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A88" s="2">
-        <v>5</v>
-      </c>
-      <c r="B88" s="3">
-        <v>44133</v>
-      </c>
+      <c r="A88" s="2"/>
+      <c r="B88" s="3"/>
       <c r="C88" s="4"/>
-      <c r="D88" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D88" s="5"/>
       <c r="E88" s="6"/>
       <c r="F88" s="6"/>
     </row>
-    <row r="89" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="5"/>
       <c r="B89" s="14"/>
-      <c r="C89" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D89" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>61</v>
-      </c>
+      <c r="C89" s="4"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="6"/>
       <c r="F89" s="4"/>
       <c r="G89" s="5"/>
       <c r="H89" s="5"/>
@@ -2648,12 +1503,8 @@
     <row r="90" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="5"/>
       <c r="B90" s="14"/>
-      <c r="C90" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D90" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C90" s="4"/>
+      <c r="D90" s="5"/>
       <c r="E90" s="17"/>
       <c r="F90" s="4"/>
       <c r="G90" s="5"/>
@@ -2675,19 +1526,13 @@
       <c r="W90" s="5"/>
       <c r="X90" s="5"/>
     </row>
-    <row r="91" spans="1:24" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A91" s="5"/>
       <c r="B91" s="14"/>
-      <c r="C91" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D91" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C91" s="4"/>
+      <c r="D91" s="5"/>
       <c r="E91" s="17"/>
-      <c r="F91" s="13" t="s">
-        <v>62</v>
-      </c>
+      <c r="F91" s="13"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
@@ -2708,196 +1553,122 @@
       <c r="X91" s="5"/>
     </row>
     <row r="92" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A92" s="15">
-        <v>1</v>
-      </c>
-      <c r="B92" s="3">
-        <v>44137</v>
-      </c>
+      <c r="A92" s="15"/>
+      <c r="B92" s="3"/>
       <c r="C92" s="4"/>
-      <c r="D92" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D92" s="5"/>
       <c r="E92" s="6"/>
       <c r="F92" s="6"/>
     </row>
-    <row r="93" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A93" s="15"/>
       <c r="B93" s="3"/>
-      <c r="C93" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D93" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>63</v>
-      </c>
+      <c r="C93" s="4"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="6"/>
       <c r="F93" s="6"/>
     </row>
     <row r="94" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="7"/>
-      <c r="C94" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D94" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C94" s="4"/>
+      <c r="D94" s="5"/>
       <c r="E94" s="6"/>
       <c r="F94" s="6"/>
     </row>
     <row r="95" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="7"/>
-      <c r="C95" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D95" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C95" s="4"/>
+      <c r="D95" s="5"/>
       <c r="E95" s="6"/>
       <c r="F95" s="6"/>
     </row>
     <row r="96" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A96" s="15">
-        <v>1</v>
-      </c>
-      <c r="B96" s="3">
-        <v>44138</v>
-      </c>
+      <c r="A96" s="15"/>
+      <c r="B96" s="3"/>
       <c r="C96" s="4"/>
-      <c r="D96" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D96" s="5"/>
       <c r="E96" s="6"/>
       <c r="F96" s="6"/>
     </row>
-    <row r="97" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A97" s="15"/>
       <c r="B97" s="3"/>
-      <c r="C97" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D97" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E97" s="6" t="s">
-        <v>64</v>
-      </c>
+      <c r="C97" s="4"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="6"/>
       <c r="F97" s="6"/>
     </row>
     <row r="98" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
       <c r="B98" s="7"/>
-      <c r="C98" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D98" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C98" s="4"/>
+      <c r="D98" s="5"/>
       <c r="E98" s="6"/>
       <c r="F98" s="6"/>
     </row>
     <row r="99" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="2"/>
       <c r="B99" s="7"/>
-      <c r="C99" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D99" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C99" s="4"/>
+      <c r="D99" s="5"/>
       <c r="E99" s="6"/>
       <c r="F99" s="6"/>
     </row>
     <row r="100" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A100" s="15">
-        <v>1</v>
-      </c>
-      <c r="B100" s="3">
-        <v>44139</v>
-      </c>
+      <c r="A100" s="15"/>
+      <c r="B100" s="3"/>
       <c r="C100" s="4"/>
-      <c r="D100" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D100" s="5"/>
       <c r="E100" s="6"/>
       <c r="F100" s="6"/>
     </row>
     <row r="101" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>
       <c r="B101" s="3"/>
-      <c r="C101" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D101" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E101" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="C101" s="4"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="6"/>
       <c r="F101" s="6"/>
     </row>
     <row r="102" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="2"/>
       <c r="B102" s="7"/>
-      <c r="C102" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D102" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C102" s="4"/>
+      <c r="D102" s="5"/>
       <c r="E102" s="6"/>
       <c r="F102" s="6"/>
     </row>
     <row r="103" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="2"/>
       <c r="B103" s="7"/>
-      <c r="C103" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D103" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C103" s="4"/>
+      <c r="D103" s="5"/>
       <c r="E103" s="6"/>
       <c r="F103" s="6"/>
     </row>
     <row r="104" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A104" s="15">
-        <v>1</v>
-      </c>
-      <c r="B104" s="3">
-        <v>44140</v>
-      </c>
+      <c r="A104" s="15"/>
+      <c r="B104" s="3"/>
       <c r="C104" s="4"/>
-      <c r="D104" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D104" s="5"/>
       <c r="E104" s="6"/>
       <c r="F104" s="6"/>
     </row>
     <row r="105" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A105" s="15"/>
       <c r="B105" s="3"/>
-      <c r="C105" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D105" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C105" s="4"/>
+      <c r="D105" s="5"/>
       <c r="E105" s="6"/>
       <c r="F105" s="6"/>
     </row>
     <row r="106" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="5"/>
       <c r="B106" s="14"/>
-      <c r="C106" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D106" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C106" s="4"/>
+      <c r="D106" s="5"/>
       <c r="E106" s="17"/>
       <c r="F106" s="4"/>
       <c r="G106" s="5"/>
@@ -2922,12 +1693,8 @@
     <row r="107" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="5"/>
       <c r="B107" s="14"/>
-      <c r="C107" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D107" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C107" s="4"/>
+      <c r="D107" s="5"/>
       <c r="E107" s="17"/>
       <c r="F107" s="4"/>
       <c r="G107" s="5"/>
@@ -2950,198 +1717,122 @@
       <c r="X107" s="5"/>
     </row>
     <row r="108" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A108" s="15">
-        <v>2</v>
-      </c>
-      <c r="B108" s="3">
-        <v>44144</v>
-      </c>
+      <c r="A108" s="15"/>
+      <c r="B108" s="3"/>
       <c r="C108" s="4"/>
-      <c r="D108" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D108" s="5"/>
       <c r="E108" s="6"/>
       <c r="F108" s="6"/>
     </row>
-    <row r="109" spans="1:24" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A109" s="15"/>
       <c r="B109" s="3"/>
-      <c r="C109" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D109" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E109" s="6" t="s">
-        <v>66</v>
-      </c>
+      <c r="C109" s="4"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="6"/>
       <c r="F109" s="6"/>
     </row>
     <row r="110" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="2"/>
       <c r="B110" s="7"/>
-      <c r="C110" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D110" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C110" s="4"/>
+      <c r="D110" s="5"/>
       <c r="E110" s="6"/>
       <c r="F110" s="6"/>
     </row>
     <row r="111" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
       <c r="B111" s="7"/>
-      <c r="C111" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D111" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C111" s="4"/>
+      <c r="D111" s="5"/>
       <c r="E111" s="6"/>
       <c r="F111" s="6"/>
     </row>
     <row r="112" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A112" s="15">
-        <v>2</v>
-      </c>
-      <c r="B112" s="3">
-        <v>44145</v>
-      </c>
+      <c r="A112" s="15"/>
+      <c r="B112" s="3"/>
       <c r="C112" s="4"/>
-      <c r="D112" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D112" s="5"/>
       <c r="E112" s="6"/>
       <c r="F112" s="6"/>
     </row>
-    <row r="113" spans="1:24" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A113" s="15"/>
       <c r="B113" s="3"/>
-      <c r="C113" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D113" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E113" s="6" t="s">
-        <v>67</v>
-      </c>
+      <c r="C113" s="4"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="6"/>
       <c r="F113" s="6"/>
     </row>
     <row r="114" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="2"/>
       <c r="B114" s="7"/>
-      <c r="C114" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D114" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C114" s="4"/>
+      <c r="D114" s="5"/>
       <c r="E114" s="6"/>
       <c r="F114" s="6"/>
     </row>
     <row r="115" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="2"/>
       <c r="B115" s="7"/>
-      <c r="C115" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D115" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C115" s="4"/>
+      <c r="D115" s="5"/>
       <c r="E115" s="6"/>
       <c r="F115" s="6"/>
     </row>
     <row r="116" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A116" s="15">
-        <v>2</v>
-      </c>
-      <c r="B116" s="3">
-        <v>44146</v>
-      </c>
+      <c r="A116" s="15"/>
+      <c r="B116" s="3"/>
       <c r="C116" s="4"/>
-      <c r="D116" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D116" s="5"/>
       <c r="E116" s="6"/>
       <c r="F116" s="6"/>
     </row>
-    <row r="117" spans="1:24" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A117" s="15"/>
       <c r="B117" s="3"/>
-      <c r="C117" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D117" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E117" s="6" t="s">
-        <v>68</v>
-      </c>
+      <c r="C117" s="13"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="6"/>
       <c r="F117" s="6"/>
     </row>
     <row r="118" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="2"/>
       <c r="B118" s="7"/>
-      <c r="C118" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D118" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C118" s="4"/>
+      <c r="D118" s="5"/>
       <c r="E118" s="6"/>
       <c r="F118" s="6"/>
     </row>
     <row r="119" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="2"/>
       <c r="B119" s="7"/>
-      <c r="C119" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D119" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C119" s="4"/>
+      <c r="D119" s="5"/>
       <c r="E119" s="6"/>
       <c r="F119" s="6"/>
     </row>
     <row r="120" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A120" s="15">
-        <v>2</v>
-      </c>
-      <c r="B120" s="3">
-        <v>44147</v>
-      </c>
+      <c r="A120" s="15"/>
+      <c r="B120" s="3"/>
       <c r="C120" s="4"/>
-      <c r="D120" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D120" s="5"/>
       <c r="E120" s="6"/>
       <c r="F120" s="6"/>
     </row>
-    <row r="121" spans="1:24" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A121" s="15"/>
       <c r="B121" s="3"/>
-      <c r="C121" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D121" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E121" s="6" t="s">
-        <v>69</v>
-      </c>
+      <c r="C121" s="13"/>
+      <c r="D121" s="5"/>
+      <c r="E121" s="6"/>
       <c r="F121" s="6"/>
     </row>
     <row r="122" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="5"/>
       <c r="B122" s="14"/>
-      <c r="C122" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D122" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C122" s="4"/>
+      <c r="D122" s="5"/>
       <c r="E122" s="17"/>
       <c r="F122" s="4"/>
       <c r="G122" s="5"/>
@@ -3166,12 +1857,8 @@
     <row r="123" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="5"/>
       <c r="B123" s="14"/>
-      <c r="C123" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D123" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C123" s="4"/>
+      <c r="D123" s="5"/>
       <c r="E123" s="17"/>
       <c r="F123" s="4"/>
       <c r="G123" s="5"/>
@@ -3194,212 +1881,130 @@
       <c r="X123" s="5"/>
     </row>
     <row r="124" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A124" s="15">
-        <v>3</v>
-      </c>
-      <c r="B124" s="3">
-        <v>44151</v>
-      </c>
+      <c r="A124" s="15"/>
+      <c r="B124" s="3"/>
       <c r="C124" s="4"/>
-      <c r="D124" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D124" s="5"/>
       <c r="E124" s="6"/>
       <c r="F124" s="6"/>
     </row>
-    <row r="125" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="2"/>
       <c r="B125" s="7"/>
-      <c r="C125" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D125" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E125" s="6" t="s">
-        <v>70</v>
-      </c>
+      <c r="C125" s="4"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="6"/>
       <c r="F125" s="6"/>
     </row>
     <row r="126" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="2"/>
       <c r="B126" s="7"/>
-      <c r="C126" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D126" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C126" s="4"/>
+      <c r="D126" s="5"/>
       <c r="E126" s="6"/>
       <c r="F126" s="6"/>
     </row>
     <row r="127" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="2"/>
       <c r="B127" s="7"/>
-      <c r="C127" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D127" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C127" s="4"/>
+      <c r="D127" s="5"/>
       <c r="E127" s="6"/>
       <c r="F127" s="6"/>
     </row>
     <row r="128" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A128" s="15">
-        <v>3</v>
-      </c>
-      <c r="B128" s="3">
-        <v>44152</v>
-      </c>
+      <c r="A128" s="15"/>
+      <c r="B128" s="3"/>
       <c r="C128" s="4"/>
-      <c r="D128" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D128" s="5"/>
       <c r="E128" s="6"/>
       <c r="F128" s="6"/>
     </row>
-    <row r="129" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A129" s="15"/>
       <c r="B129" s="3"/>
-      <c r="C129" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D129" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E129" s="6" t="s">
-        <v>71</v>
-      </c>
+      <c r="C129" s="4"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="6"/>
       <c r="F129" s="6"/>
     </row>
     <row r="130" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="2"/>
       <c r="B130" s="7"/>
-      <c r="C130" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D130" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C130" s="4"/>
+      <c r="D130" s="5"/>
       <c r="E130" s="6"/>
       <c r="F130" s="6"/>
     </row>
     <row r="131" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="2"/>
       <c r="B131" s="7"/>
-      <c r="C131" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D131" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C131" s="4"/>
+      <c r="D131" s="5"/>
       <c r="E131" s="6"/>
       <c r="F131" s="6"/>
     </row>
     <row r="132" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A132" s="15">
-        <v>3</v>
-      </c>
-      <c r="B132" s="3">
-        <v>44153</v>
-      </c>
+      <c r="A132" s="15"/>
+      <c r="B132" s="3"/>
       <c r="C132" s="4"/>
-      <c r="D132" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D132" s="5"/>
       <c r="E132" s="6"/>
       <c r="F132" s="6"/>
     </row>
-    <row r="133" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A133" s="15"/>
       <c r="B133" s="3"/>
-      <c r="C133" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D133" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E133" s="6" t="s">
-        <v>72</v>
-      </c>
+      <c r="C133" s="13"/>
+      <c r="D133" s="5"/>
+      <c r="E133" s="6"/>
       <c r="F133" s="6"/>
     </row>
     <row r="134" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A134" s="15"/>
       <c r="B134" s="3"/>
-      <c r="C134" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D134" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E134" s="18" t="s">
-        <v>73</v>
-      </c>
+      <c r="C134" s="13"/>
+      <c r="D134" s="5"/>
+      <c r="E134" s="18"/>
       <c r="F134" s="6"/>
     </row>
     <row r="135" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="2"/>
       <c r="B135" s="7"/>
-      <c r="C135" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D135" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C135" s="4"/>
+      <c r="D135" s="5"/>
       <c r="E135" s="6"/>
       <c r="F135" s="6"/>
     </row>
     <row r="136" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="2"/>
       <c r="B136" s="7"/>
-      <c r="C136" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D136" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C136" s="4"/>
+      <c r="D136" s="5"/>
       <c r="E136" s="6"/>
       <c r="F136" s="6"/>
     </row>
     <row r="137" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A137" s="15">
-        <v>3</v>
-      </c>
-      <c r="B137" s="3">
-        <v>44154</v>
-      </c>
+      <c r="A137" s="15"/>
+      <c r="B137" s="3"/>
       <c r="C137" s="4"/>
-      <c r="D137" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D137" s="5"/>
       <c r="E137" s="6"/>
       <c r="F137" s="6"/>
     </row>
-    <row r="138" spans="1:24" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A138" s="15"/>
       <c r="B138" s="3"/>
-      <c r="C138" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D138" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E138" s="13" t="s">
-        <v>75</v>
-      </c>
+      <c r="C138" s="13"/>
+      <c r="D138" s="5"/>
+      <c r="E138" s="13"/>
       <c r="F138" s="6"/>
     </row>
     <row r="139" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="5"/>
       <c r="B139" s="14"/>
-      <c r="C139" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D139" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C139" s="4"/>
+      <c r="D139" s="5"/>
       <c r="E139" s="17"/>
       <c r="F139" s="4"/>
       <c r="G139" s="5"/>
@@ -3424,12 +2029,8 @@
     <row r="140" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="5"/>
       <c r="B140" s="14"/>
-      <c r="C140" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D140" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C140" s="4"/>
+      <c r="D140" s="5"/>
       <c r="E140" s="17"/>
       <c r="F140" s="4"/>
       <c r="G140" s="5"/>
@@ -3451,217 +2052,131 @@
       <c r="W140" s="5"/>
       <c r="X140" s="5"/>
     </row>
-    <row r="141" spans="1:24" ht="114" x14ac:dyDescent="0.2">
-      <c r="A141" s="15">
-        <v>4</v>
-      </c>
-      <c r="B141" s="3">
-        <v>44158</v>
-      </c>
-      <c r="C141" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D141" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E141" s="13" t="s">
-        <v>76</v>
-      </c>
+    <row r="141" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A141" s="15"/>
+      <c r="B141" s="3"/>
+      <c r="C141" s="13"/>
+      <c r="D141" s="5"/>
+      <c r="E141" s="13"/>
       <c r="F141" s="6"/>
     </row>
-    <row r="142" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A142" s="15"/>
       <c r="B142" s="3"/>
-      <c r="C142" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D142" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E142" s="13" t="s">
-        <v>77</v>
-      </c>
+      <c r="C142" s="13"/>
+      <c r="D142" s="5"/>
+      <c r="E142" s="13"/>
       <c r="F142" s="6"/>
     </row>
     <row r="143" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="2"/>
       <c r="B143" s="7"/>
-      <c r="C143" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D143" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C143" s="4"/>
+      <c r="D143" s="5"/>
       <c r="E143" s="6"/>
       <c r="F143" s="6"/>
     </row>
     <row r="144" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="2"/>
       <c r="B144" s="7"/>
-      <c r="C144" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D144" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C144" s="4"/>
+      <c r="D144" s="5"/>
       <c r="E144" s="6"/>
       <c r="F144" s="6"/>
     </row>
     <row r="145" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A145" s="15">
-        <v>4</v>
-      </c>
-      <c r="B145" s="3">
-        <v>44159</v>
-      </c>
+      <c r="A145" s="15"/>
+      <c r="B145" s="3"/>
       <c r="C145" s="4"/>
-      <c r="D145" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D145" s="5"/>
       <c r="E145" s="6"/>
       <c r="F145" s="6"/>
     </row>
     <row r="146" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A146" s="15"/>
       <c r="B146" s="3"/>
-      <c r="C146" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D146" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E146" s="13" t="s">
-        <v>78</v>
-      </c>
+      <c r="C146" s="13"/>
+      <c r="D146" s="5"/>
+      <c r="E146" s="13"/>
       <c r="F146" s="6"/>
     </row>
     <row r="147" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A147" s="2"/>
       <c r="B147" s="7"/>
-      <c r="C147" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D147" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E147" s="13" t="s">
-        <v>79</v>
-      </c>
+      <c r="C147" s="13"/>
+      <c r="D147" s="5"/>
+      <c r="E147" s="13"/>
       <c r="F147" s="6"/>
     </row>
     <row r="148" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="2"/>
       <c r="B148" s="7"/>
-      <c r="C148" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D148" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C148" s="4"/>
+      <c r="D148" s="5"/>
       <c r="E148" s="6"/>
       <c r="F148" s="6"/>
     </row>
     <row r="149" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A149" s="2"/>
       <c r="B149" s="7"/>
-      <c r="C149" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D149" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C149" s="4"/>
+      <c r="D149" s="5"/>
       <c r="E149" s="6"/>
       <c r="F149" s="6"/>
     </row>
     <row r="150" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A150" s="15">
-        <v>4</v>
-      </c>
-      <c r="B150" s="3">
-        <v>44160</v>
-      </c>
+      <c r="A150" s="15"/>
+      <c r="B150" s="3"/>
       <c r="C150" s="4"/>
-      <c r="D150" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D150" s="5"/>
       <c r="E150" s="6"/>
       <c r="F150" s="6"/>
     </row>
-    <row r="151" spans="1:24" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A151" s="15"/>
       <c r="B151" s="3"/>
-      <c r="C151" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D151" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E151" s="13" t="s">
-        <v>80</v>
-      </c>
+      <c r="C151" s="13"/>
+      <c r="D151" s="5"/>
+      <c r="E151" s="13"/>
       <c r="F151" s="6"/>
     </row>
     <row r="152" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="2"/>
       <c r="B152" s="7"/>
-      <c r="C152" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D152" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C152" s="4"/>
+      <c r="D152" s="5"/>
       <c r="E152" s="6"/>
       <c r="F152" s="6"/>
     </row>
     <row r="153" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="2"/>
       <c r="B153" s="7"/>
-      <c r="C153" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D153" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C153" s="4"/>
+      <c r="D153" s="5"/>
       <c r="E153" s="6"/>
       <c r="F153" s="6"/>
     </row>
     <row r="154" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A154" s="15">
-        <v>4</v>
-      </c>
-      <c r="B154" s="3">
-        <v>44161</v>
-      </c>
+      <c r="A154" s="15"/>
+      <c r="B154" s="3"/>
       <c r="C154" s="4"/>
-      <c r="D154" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D154" s="5"/>
       <c r="E154" s="6"/>
       <c r="F154" s="6"/>
     </row>
-    <row r="155" spans="1:24" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A155" s="15"/>
       <c r="B155" s="3"/>
-      <c r="C155" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D155" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E155" s="13" t="s">
-        <v>81</v>
-      </c>
+      <c r="C155" s="13"/>
+      <c r="D155" s="5"/>
+      <c r="E155" s="13"/>
       <c r="F155" s="6"/>
     </row>
     <row r="156" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="5"/>
       <c r="B156" s="14"/>
-      <c r="C156" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D156" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C156" s="4"/>
+      <c r="D156" s="5"/>
       <c r="E156" s="17"/>
       <c r="F156" s="4"/>
       <c r="G156" s="5"/>
@@ -3686,12 +2201,8 @@
     <row r="157" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A157" s="5"/>
       <c r="B157" s="14"/>
-      <c r="C157" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D157" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C157" s="4"/>
+      <c r="D157" s="5"/>
       <c r="E157" s="17"/>
       <c r="F157" s="4"/>
       <c r="G157" s="5"/>
@@ -3714,210 +2225,130 @@
       <c r="X157" s="5"/>
     </row>
     <row r="158" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A158" s="15">
-        <v>5</v>
-      </c>
-      <c r="B158" s="3">
-        <v>44165</v>
-      </c>
+      <c r="A158" s="15"/>
+      <c r="B158" s="3"/>
       <c r="C158" s="4"/>
-      <c r="D158" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D158" s="5"/>
       <c r="E158" s="6"/>
       <c r="F158" s="6"/>
     </row>
     <row r="159" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A159" s="2"/>
       <c r="B159" s="7"/>
-      <c r="C159" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D159" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E159" s="13" t="s">
-        <v>82</v>
-      </c>
+      <c r="C159" s="13"/>
+      <c r="D159" s="5"/>
+      <c r="E159" s="13"/>
       <c r="F159" s="6"/>
     </row>
     <row r="160" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A160" s="2"/>
       <c r="B160" s="7"/>
-      <c r="C160" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D160" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C160" s="4"/>
+      <c r="D160" s="5"/>
       <c r="E160" s="6"/>
       <c r="F160" s="6"/>
     </row>
     <row r="161" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A161" s="2"/>
       <c r="B161" s="7"/>
-      <c r="C161" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D161" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C161" s="4"/>
+      <c r="D161" s="5"/>
       <c r="E161" s="6"/>
       <c r="F161" s="6"/>
     </row>
     <row r="162" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A162" s="15">
-        <v>1</v>
-      </c>
-      <c r="B162" s="3">
-        <v>44166</v>
-      </c>
+      <c r="A162" s="15"/>
+      <c r="B162" s="3"/>
       <c r="C162" s="4"/>
-      <c r="D162" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D162" s="5"/>
       <c r="E162" s="6"/>
       <c r="F162" s="6"/>
     </row>
-    <row r="163" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A163" s="2"/>
       <c r="B163" s="7"/>
-      <c r="C163" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D163" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E163" s="19" t="s">
-        <v>83</v>
-      </c>
+      <c r="C163" s="4"/>
+      <c r="D163" s="5"/>
+      <c r="E163" s="19"/>
       <c r="F163" s="6"/>
     </row>
     <row r="164" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A164" s="2"/>
       <c r="B164" s="7"/>
-      <c r="C164" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D164" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C164" s="4"/>
+      <c r="D164" s="5"/>
       <c r="E164" s="6"/>
       <c r="F164" s="6"/>
     </row>
     <row r="165" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A165" s="2"/>
       <c r="B165" s="7"/>
-      <c r="C165" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D165" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C165" s="4"/>
+      <c r="D165" s="5"/>
       <c r="E165" s="6"/>
       <c r="F165" s="6"/>
     </row>
     <row r="166" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A166" s="15">
-        <v>1</v>
-      </c>
-      <c r="B166" s="3">
-        <v>44167</v>
-      </c>
+      <c r="A166" s="15"/>
+      <c r="B166" s="3"/>
       <c r="C166" s="4"/>
-      <c r="D166" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D166" s="5"/>
       <c r="E166" s="6"/>
       <c r="F166" s="6"/>
     </row>
     <row r="167" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A167" s="15"/>
       <c r="B167" s="3"/>
-      <c r="C167" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D167" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C167" s="13"/>
+      <c r="D167" s="5"/>
       <c r="E167" s="6"/>
       <c r="F167" s="6"/>
     </row>
     <row r="168" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A168" s="2"/>
       <c r="B168" s="7"/>
-      <c r="C168" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D168" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C168" s="4"/>
+      <c r="D168" s="5"/>
       <c r="E168" s="6"/>
       <c r="F168" s="6"/>
     </row>
     <row r="169" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A169" s="2"/>
       <c r="B169" s="7"/>
-      <c r="C169" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D169" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C169" s="4"/>
+      <c r="D169" s="5"/>
       <c r="E169" s="6"/>
       <c r="F169" s="6"/>
     </row>
     <row r="170" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A170" s="15">
-        <v>1</v>
-      </c>
-      <c r="B170" s="3">
-        <v>44168</v>
-      </c>
+      <c r="A170" s="15"/>
+      <c r="B170" s="3"/>
       <c r="C170" s="4"/>
-      <c r="D170" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D170" s="5"/>
       <c r="E170" s="6"/>
       <c r="F170" s="6"/>
     </row>
     <row r="171" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A171" s="15"/>
       <c r="B171" s="3"/>
-      <c r="C171" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D171" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E171" s="13" t="s">
-        <v>85</v>
-      </c>
+      <c r="C171" s="13"/>
+      <c r="D171" s="5"/>
+      <c r="E171" s="13"/>
       <c r="F171" s="6"/>
     </row>
-    <row r="172" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A172" s="15"/>
       <c r="B172" s="3"/>
-      <c r="C172" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D172" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E172" s="13" t="s">
-        <v>86</v>
-      </c>
+      <c r="C172" s="13"/>
+      <c r="D172" s="5"/>
+      <c r="E172" s="13"/>
       <c r="F172" s="6"/>
     </row>
     <row r="173" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A173" s="5"/>
       <c r="B173" s="14"/>
-      <c r="C173" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D173" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C173" s="4"/>
+      <c r="D173" s="5"/>
       <c r="E173" s="17"/>
       <c r="F173" s="4"/>
       <c r="G173" s="5"/>
@@ -3942,12 +2373,8 @@
     <row r="174" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A174" s="5"/>
       <c r="B174" s="14"/>
-      <c r="C174" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D174" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C174" s="4"/>
+      <c r="D174" s="5"/>
       <c r="E174" s="17"/>
       <c r="F174" s="4"/>
       <c r="G174" s="5"/>
@@ -3970,212 +2397,130 @@
       <c r="X174" s="5"/>
     </row>
     <row r="175" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A175" s="15">
-        <v>2</v>
-      </c>
-      <c r="B175" s="3">
-        <v>44172</v>
-      </c>
+      <c r="A175" s="15"/>
+      <c r="B175" s="3"/>
       <c r="C175" s="4"/>
-      <c r="D175" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D175" s="5"/>
       <c r="E175" s="6"/>
       <c r="F175" s="6"/>
     </row>
-    <row r="176" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A176" s="15"/>
       <c r="B176" s="3"/>
-      <c r="C176" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D176" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E176" s="6" t="s">
-        <v>87</v>
-      </c>
+      <c r="C176" s="4"/>
+      <c r="D176" s="5"/>
+      <c r="E176" s="6"/>
       <c r="F176" s="6"/>
     </row>
     <row r="177" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A177" s="2"/>
       <c r="B177" s="7"/>
-      <c r="C177" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D177" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C177" s="4"/>
+      <c r="D177" s="5"/>
       <c r="E177" s="6"/>
       <c r="F177" s="6"/>
     </row>
     <row r="178" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A178" s="2"/>
       <c r="B178" s="7"/>
-      <c r="C178" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D178" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C178" s="4"/>
+      <c r="D178" s="5"/>
       <c r="E178" s="6"/>
       <c r="F178" s="6"/>
     </row>
     <row r="179" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A179" s="15">
-        <v>2</v>
-      </c>
-      <c r="B179" s="3">
-        <v>44173</v>
-      </c>
+      <c r="A179" s="15"/>
+      <c r="B179" s="3"/>
       <c r="C179" s="4"/>
-      <c r="D179" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D179" s="5"/>
       <c r="E179" s="6"/>
       <c r="F179" s="6"/>
     </row>
-    <row r="180" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A180" s="15"/>
       <c r="B180" s="3"/>
-      <c r="C180" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D180" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E180" s="6" t="s">
-        <v>88</v>
-      </c>
+      <c r="C180" s="4"/>
+      <c r="D180" s="5"/>
+      <c r="E180" s="6"/>
       <c r="F180" s="6"/>
     </row>
     <row r="181" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A181" s="2"/>
       <c r="B181" s="7"/>
-      <c r="C181" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D181" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C181" s="4"/>
+      <c r="D181" s="5"/>
       <c r="E181" s="6"/>
       <c r="F181" s="6"/>
     </row>
     <row r="182" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A182" s="2"/>
       <c r="B182" s="7"/>
-      <c r="C182" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D182" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C182" s="4"/>
+      <c r="D182" s="5"/>
       <c r="E182" s="6"/>
       <c r="F182" s="6"/>
     </row>
     <row r="183" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A183" s="15">
-        <v>2</v>
-      </c>
-      <c r="B183" s="3">
-        <v>44174</v>
-      </c>
+      <c r="A183" s="15"/>
+      <c r="B183" s="3"/>
       <c r="C183" s="4"/>
-      <c r="D183" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D183" s="5"/>
       <c r="E183" s="6"/>
       <c r="F183" s="6"/>
     </row>
-    <row r="184" spans="1:24" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A184" s="15"/>
       <c r="B184" s="3"/>
-      <c r="C184" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D184" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E184" s="13" t="s">
-        <v>89</v>
-      </c>
+      <c r="C184" s="13"/>
+      <c r="D184" s="5"/>
+      <c r="E184" s="13"/>
       <c r="F184" s="6"/>
     </row>
     <row r="185" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A185" s="2"/>
       <c r="B185" s="7"/>
-      <c r="C185" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D185" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C185" s="4"/>
+      <c r="D185" s="5"/>
       <c r="E185" s="6"/>
       <c r="F185" s="6"/>
     </row>
     <row r="186" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A186" s="2"/>
       <c r="B186" s="7"/>
-      <c r="C186" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D186" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C186" s="4"/>
+      <c r="D186" s="5"/>
       <c r="E186" s="6"/>
       <c r="F186" s="6"/>
     </row>
     <row r="187" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A187" s="15">
-        <v>2</v>
-      </c>
-      <c r="B187" s="3">
-        <v>44175</v>
-      </c>
+      <c r="A187" s="15"/>
+      <c r="B187" s="3"/>
       <c r="C187" s="4"/>
-      <c r="D187" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D187" s="5"/>
       <c r="E187" s="6"/>
       <c r="F187" s="6"/>
     </row>
-    <row r="188" spans="1:24" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A188" s="15"/>
       <c r="B188" s="3"/>
-      <c r="C188" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D188" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E188" s="13" t="s">
-        <v>90</v>
-      </c>
+      <c r="C188" s="13"/>
+      <c r="D188" s="5"/>
+      <c r="E188" s="13"/>
       <c r="F188" s="6"/>
     </row>
-    <row r="189" spans="1:24" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A189" s="15"/>
       <c r="B189" s="3"/>
-      <c r="C189" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D189" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E189" s="13" t="s">
-        <v>91</v>
-      </c>
+      <c r="C189" s="13"/>
+      <c r="D189" s="5"/>
+      <c r="E189" s="13"/>
       <c r="F189" s="6"/>
     </row>
     <row r="190" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A190" s="5"/>
       <c r="B190" s="14"/>
-      <c r="C190" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D190" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C190" s="4"/>
+      <c r="D190" s="5"/>
       <c r="E190" s="17"/>
       <c r="F190" s="4"/>
       <c r="G190" s="5"/>
@@ -4200,12 +2545,8 @@
     <row r="191" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A191" s="5"/>
       <c r="B191" s="14"/>
-      <c r="C191" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D191" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C191" s="4"/>
+      <c r="D191" s="5"/>
       <c r="E191" s="17"/>
       <c r="F191" s="4"/>
       <c r="G191" s="5"/>
@@ -4228,186 +2569,114 @@
       <c r="X191" s="5"/>
     </row>
     <row r="192" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A192" s="15">
-        <v>3</v>
-      </c>
-      <c r="B192" s="3">
-        <v>44179</v>
-      </c>
+      <c r="A192" s="15"/>
+      <c r="B192" s="3"/>
       <c r="C192" s="4"/>
-      <c r="D192" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D192" s="5"/>
       <c r="E192" s="6"/>
       <c r="F192" s="6"/>
     </row>
-    <row r="193" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A193" s="15"/>
       <c r="B193" s="3"/>
-      <c r="C193" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D193" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E193" s="13" t="s">
-        <v>92</v>
-      </c>
+      <c r="C193" s="13"/>
+      <c r="D193" s="5"/>
+      <c r="E193" s="13"/>
       <c r="F193" s="6"/>
     </row>
     <row r="194" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A194" s="2"/>
       <c r="B194" s="7"/>
-      <c r="C194" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D194" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C194" s="4"/>
+      <c r="D194" s="5"/>
       <c r="E194" s="6"/>
       <c r="F194" s="6"/>
     </row>
     <row r="195" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A195" s="2"/>
       <c r="B195" s="7"/>
-      <c r="C195" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D195" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C195" s="4"/>
+      <c r="D195" s="5"/>
       <c r="E195" s="6"/>
       <c r="F195" s="6"/>
     </row>
     <row r="196" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A196" s="15">
-        <v>3</v>
-      </c>
-      <c r="B196" s="3">
-        <v>44180</v>
-      </c>
+      <c r="A196" s="15"/>
+      <c r="B196" s="3"/>
       <c r="C196" s="4"/>
-      <c r="D196" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D196" s="5"/>
       <c r="E196" s="6"/>
       <c r="F196" s="6"/>
     </row>
-    <row r="197" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A197" s="15"/>
       <c r="B197" s="3"/>
-      <c r="C197" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D197" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E197" s="13" t="s">
-        <v>93</v>
-      </c>
+      <c r="C197" s="13"/>
+      <c r="D197" s="5"/>
+      <c r="E197" s="13"/>
       <c r="F197" s="6"/>
     </row>
     <row r="198" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A198" s="2"/>
       <c r="B198" s="7"/>
-      <c r="C198" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D198" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C198" s="4"/>
+      <c r="D198" s="5"/>
       <c r="E198" s="6"/>
       <c r="F198" s="6"/>
     </row>
     <row r="199" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A199" s="2"/>
       <c r="B199" s="7"/>
-      <c r="C199" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D199" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C199" s="4"/>
+      <c r="D199" s="5"/>
       <c r="E199" s="6"/>
       <c r="F199" s="6"/>
     </row>
     <row r="200" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A200" s="15">
-        <v>3</v>
-      </c>
-      <c r="B200" s="3">
-        <v>44181</v>
-      </c>
+      <c r="A200" s="15"/>
+      <c r="B200" s="3"/>
       <c r="C200" s="4"/>
-      <c r="D200" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="D200" s="5"/>
       <c r="E200" s="6"/>
       <c r="F200" s="6"/>
     </row>
-    <row r="201" spans="1:24" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A201" s="15"/>
       <c r="B201" s="3"/>
-      <c r="C201" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D201" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E201" s="13" t="s">
-        <v>94</v>
-      </c>
+      <c r="C201" s="13"/>
+      <c r="D201" s="5"/>
+      <c r="E201" s="13"/>
       <c r="F201" s="6"/>
     </row>
     <row r="202" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A202" s="2"/>
       <c r="B202" s="7"/>
-      <c r="C202" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D202" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C202" s="4"/>
+      <c r="D202" s="5"/>
       <c r="E202" s="6"/>
       <c r="F202" s="6"/>
     </row>
     <row r="203" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A203" s="2"/>
       <c r="B203" s="7"/>
-      <c r="C203" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D203" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C203" s="4"/>
+      <c r="D203" s="5"/>
       <c r="E203" s="6"/>
       <c r="F203" s="6"/>
     </row>
     <row r="204" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A204" s="15">
-        <v>3</v>
-      </c>
-      <c r="B204" s="3">
-        <v>44182</v>
-      </c>
+      <c r="A204" s="15"/>
+      <c r="B204" s="3"/>
       <c r="C204" s="4"/>
-      <c r="D204" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E204" s="20" t="s">
-        <v>95</v>
-      </c>
+      <c r="D204" s="5"/>
+      <c r="E204" s="20"/>
       <c r="F204" s="6"/>
     </row>
     <row r="205" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A205" s="5"/>
       <c r="B205" s="14"/>
-      <c r="C205" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D205" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C205" s="4"/>
+      <c r="D205" s="5"/>
       <c r="E205" s="17"/>
       <c r="F205" s="4"/>
       <c r="G205" s="5"/>
@@ -4432,12 +2701,8 @@
     <row r="206" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A206" s="5"/>
       <c r="B206" s="14"/>
-      <c r="C206" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D206" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="C206" s="4"/>
+      <c r="D206" s="5"/>
       <c r="E206" s="17"/>
       <c r="F206" s="4"/>
       <c r="G206" s="5"/>
@@ -13240,11 +11505,6 @@
       <c r="F1084" s="6"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E26" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E163" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -13302,7 +11562,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
@@ -13332,32 +11592,32 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -13381,7 +11641,7 @@
         <v>43840</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="C1" s="5">
         <v>7.5</v>
@@ -13392,7 +11652,7 @@
         <v>43871</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>98</v>
+        <v>25</v>
       </c>
       <c r="C2" s="5">
         <v>2</v>
@@ -13403,7 +11663,7 @@
         <v>43900</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="C3" s="5">
         <v>0</v>
@@ -13414,7 +11674,7 @@
         <v>43931</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="C4" s="5">
         <v>3</v>
@@ -13425,7 +11685,7 @@
         <v>43961</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="C5" s="5">
         <v>6.5</v>
@@ -13436,14 +11696,14 @@
         <v>43992</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="C6" s="5">
         <f>1+2+1.5+2</f>
         <v>6.5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -13451,7 +11711,7 @@
         <v>44022</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="C7" s="5">
         <f>0.8+2+1.5+2.5</f>
@@ -13463,7 +11723,7 @@
         <v>44053</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="C8" s="5">
         <f>(15/60)+3+1+(15/60)+2</f>
@@ -13515,7 +11775,7 @@
         <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E1" s="5" t="b">
         <v>1</v>
@@ -13524,7 +11784,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="11">

</xml_diff>